<commit_message>
Added issues, also closes #10
</commit_message>
<xml_diff>
--- a/Documentation/Issue Tracking/Issue Tracking.xlsx
+++ b/Documentation/Issue Tracking/Issue Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Issue Name</t>
   </si>
@@ -61,14 +61,67 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Project Risk Management Plan</t>
+  </si>
+  <si>
+    <t>Risk management plan has been reviewed by the team and subsequently this issue/task is closed.</t>
+  </si>
+  <si>
+    <t>Why Android</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Target Audience</t>
+  </si>
+  <si>
+    <t>Stakeholder Analysis</t>
+  </si>
+  <si>
+    <t>Completed document</t>
+  </si>
+  <si>
+    <t>Document describing how we will manage risks faced by the project</t>
+  </si>
+  <si>
+    <t>Document describing why we chose to develop for the android operating system</t>
+  </si>
+  <si>
+    <t>Document describing our target audience</t>
+  </si>
+  <si>
+    <t>Document describing the various stakeholders of the project and our strategy for them</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,13 +149,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -123,16 +216,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -141,6 +224,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:J1048576"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Issue #" dataDxfId="3"/>
+    <tableColumn id="2" name="Issue Name"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Created By"/>
+    <tableColumn id="5" name="Assigned To"/>
+    <tableColumn id="6" name="Start Date"/>
+    <tableColumn id="7" name="End Date"/>
+    <tableColumn id="8" name="Description" dataDxfId="2"/>
+    <tableColumn id="9" name="Status"/>
+    <tableColumn id="10" name="Resolution" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,7 +532,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -438,80 +540,229 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="3"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="8" max="8" width="43.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="89.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K2" t="s">
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1">
+        <v>41897</v>
+      </c>
+      <c r="G2" s="1">
+        <v>41907</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>41897</v>
+      </c>
+      <c r="G3" s="1">
+        <v>41909</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
         <v>11</v>
       </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K4" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>41897</v>
+      </c>
+      <c r="G4" s="1">
+        <v>41909</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
         <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>41896</v>
+      </c>
+      <c r="G5" s="1">
+        <v>41910</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="I2:I1048576">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Open"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 D2:D1048576">
-      <formula1>$K$1:$K$4</formula1>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E1048576">
+      <formula1>$L$1:$L$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
-      <formula1>$L$1:$L$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+      <formula1>$M$1:$M$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+      <formula1>$N$2:$N$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>